<commit_message>
NW final work push
</commit_message>
<xml_diff>
--- a/year by month cumulative.xlsx
+++ b/year by month cumulative.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicole Wittlin.000\Documents\Classes\APRA Data Viz Challenge\github\APRA-DataViz-Challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457AAC05-CD59-4253-A623-2C8152A2CD5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F1D7DE-E2EC-4755-B5D0-AA183023147D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{5A8A56EC-438E-43ED-B1D4-3D39B175AD45}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="2" xr2:uid="{5A8A56EC-438E-43ED-B1D4-3D39B175AD45}"/>
   </bookViews>
   <sheets>
     <sheet name="Month by Month" sheetId="1" r:id="rId1"/>
@@ -2021,7 +2021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{138C7AF6-B09A-43B2-8147-A1BA74F1266B}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -2298,7 +2298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B38909-D706-41D0-95DA-2313B39124DE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>

</xml_diff>